<commit_message>
Added simple folders for simple coding and art
</commit_message>
<xml_diff>
--- a/Group 12 Plan.xlsx
+++ b/Group 12 Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ccdd44787473a730/Desktop/Louisiana Tech/First Year/Thired Quarter (2020-Freshman)/Computer Sci 3/GitHub/Team Project/2020CompSci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{B1870092-A533-47C2-9F0F-86D8E6F9D14D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2048FA32-C125-41E6-B2AE-41B1F1E70049}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{B1870092-A533-47C2-9F0F-86D8E6F9D14D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{63AA99E2-0043-4999-826A-E7A42B8A8CD5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{15D89691-9E01-481F-A18B-41883EF0F508}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Group 12 Plan</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>Due</t>
-  </si>
-  <si>
-    <t>3D engine</t>
   </si>
   <si>
     <t>Main Job</t>
@@ -536,7 +533,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,13 +585,13 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="15"/>
@@ -603,14 +600,14 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
       <c r="H7" s="2"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
@@ -618,29 +615,29 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="2"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="16"/>
+      <c r="G9" s="4"/>
       <c r="H9" s="16"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
@@ -648,56 +645,68 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="4"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="4"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>18</v>
+      <c r="B12" s="3">
+        <v>43913</v>
+      </c>
+      <c r="C12" s="3">
+        <v>43920</v>
+      </c>
+      <c r="D12" s="3">
+        <v>43927</v>
+      </c>
+      <c r="E12" s="3">
+        <v>43934</v>
+      </c>
+      <c r="F12" s="3">
+        <v>43941</v>
+      </c>
+      <c r="G12" s="3">
+        <v>43948</v>
+      </c>
+      <c r="H12" s="3">
+        <v>43952</v>
       </c>
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
@@ -706,28 +715,6 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3">
-        <v>43913</v>
-      </c>
-      <c r="C13" s="3">
-        <v>43920</v>
-      </c>
-      <c r="D13" s="3">
-        <v>43927</v>
-      </c>
-      <c r="E13" s="3">
-        <v>43934</v>
-      </c>
-      <c r="F13" s="3">
-        <v>43941</v>
-      </c>
-      <c r="G13" s="3">
-        <v>43948</v>
-      </c>
-      <c r="H13" s="3">
-        <v>43952</v>
-      </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
     </row>
@@ -736,7 +723,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -744,7 +731,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -752,7 +739,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -760,7 +747,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -784,7 +771,7 @@
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
@@ -793,7 +780,7 @@
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>

</xml_diff>